<commit_message>
integrating Matt's edits, starting read-through
</commit_message>
<xml_diff>
--- a/Documents/author_information.xlsx
+++ b/Documents/author_information.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atyler/Documents/Projects/Islets/manuscripts/HighDimensionalMediation/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C573C47-B13F-F446-9794-2A9D9C87A82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF305B5-2346-B24C-A21F-1716D809C8E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{DE77C90A-4A6B-FA47-B2CD-2FDE87027E11}"/>
   </bookViews>
@@ -596,7 +596,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updates responding to reviewers
</commit_message>
<xml_diff>
--- a/Documents/author_information.xlsx
+++ b/Documents/author_information.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atyler/Documents/Projects/Islets/manuscripts/HighDimensionalMediation/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF305B5-2346-B24C-A21F-1716D809C8E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43161821-6B93-3049-81E9-238116FB8B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{DE77C90A-4A6B-FA47-B2CD-2FDE87027E11}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="45">
   <si>
     <t>Anna L. Tyler</t>
   </si>
@@ -156,6 +156,21 @@
   </si>
   <si>
     <t>0000-0001-9190-9284</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>207-288-6000</t>
+  </si>
+  <si>
+    <t>608-262-1372</t>
+  </si>
+  <si>
+    <t>433 Babcock Drive</t>
+  </si>
+  <si>
+    <t>isabela.gyuricza@jax.org</t>
   </si>
 </sst>
 </file>
@@ -241,10 +256,9 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -258,6 +272,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -593,193 +608,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24EF319-CC4A-FE4A-B4BC-A6EB11A663F6}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="48.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="E1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="D2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
+      <c r="D3" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
+      <c r="E4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4">
+        <v>53706</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="D5" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="D7" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="4" t="s">
+      <c r="B8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="D8" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+      <c r="D10" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="D12" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>18</v>
       </c>
     </row>
@@ -797,6 +829,8 @@
     <hyperlink ref="C7" r:id="rId10" display="https://orcid.org/0000-0002-8455-3993" xr:uid="{22A79ECB-73B6-064B-89E2-B6B99631E9BC}"/>
     <hyperlink ref="C8" r:id="rId11" display="https://orcid.org/0000-0002-7969-1910" xr:uid="{D6C6B333-45D1-0249-9BD2-DFE4EBCA74E8}"/>
     <hyperlink ref="C10" r:id="rId12" display="https://orcid.org/0000-0002-7599-7365" xr:uid="{5D1579A1-55FF-D045-81DD-A865649CFC1E}"/>
+    <hyperlink ref="E4" r:id="rId13" display="tel:(608) 262-1372" xr:uid="{4DD53C84-5EC0-0445-8032-BA191A194A9A}"/>
+    <hyperlink ref="B8" r:id="rId14" xr:uid="{68509614-4477-7D46-8295-92E93C2FB05A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>